<commit_message>
test: Add RIASEC scoring test script
</commit_message>
<xml_diff>
--- a/New RIASEC/RIASEC_Master_Global_Bilingual.xlsx
+++ b/New RIASEC/RIASEC_Master_Global_Bilingual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mona-Yashar\school2career-15-9-2025 - Copy - KIRO\New RIASEC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E956746D-EA21-472C-82C3-C05B918E5131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB8E52D-8AE2-419E-838B-070ED7DBC6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegionMap" sheetId="1" r:id="rId1"/>
@@ -5546,12 +5546,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -5581,7 +5587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5589,6 +5595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20091,7 +20098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -23626,9 +23633,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="173.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="129.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="184.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="132.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="245.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="168.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="242.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="176.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -23688,32 +23708,32 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>1232</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>1233</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>285</v>
       </c>
     </row>

</xml_diff>